<commit_message>
Update Day 21 spreadsheet
</commit_message>
<xml_diff>
--- a/AOC/Year2018/Day21/Day21.xlsx
+++ b/AOC/Year2018/Day21/Day21.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\adventofcode2018\AOC\Year2018\Day21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{872AF544-63D6-411E-BF4A-4BCCE8E5B231}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C25E0B-1D08-45C8-8C31-45DF1BE982EA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18525" windowHeight="11483" xr2:uid="{CDDEAB3D-D7A5-4A1F-AA8E-A5CC30FAEF9D}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="64">
   <si>
     <t>#ip 3</t>
   </si>
@@ -162,21 +162,18 @@
     <t>r4 *= 65899</t>
   </si>
   <si>
-    <t>r5 = 256 == r1 ? 1 : 0</t>
-  </si>
-  <si>
     <t>IP += r5</t>
   </si>
   <si>
+    <t>IP += r2</t>
+  </si>
+  <si>
     <t>IP ++</t>
   </si>
   <si>
     <t>GOTO 28</t>
   </si>
   <si>
-    <t>if r1 == 256 then GOTO 28 else GOTO 17</t>
-  </si>
-  <si>
     <t>r5 = 0</t>
   </si>
   <si>
@@ -187,6 +184,45 @@
   </si>
   <si>
     <t>r2 = r2 &gt; r1 ? 1 : 0</t>
+  </si>
+  <si>
+    <t>GOTO 26</t>
+  </si>
+  <si>
+    <t>if r2 &gt; r1 then GOTO 26 else GOTO 24</t>
+  </si>
+  <si>
+    <t>r5++</t>
+  </si>
+  <si>
+    <t>r1 = r5</t>
+  </si>
+  <si>
+    <t>GOTO 8</t>
+  </si>
+  <si>
+    <t>r5 = r4 == r0 ? 1 : 0</t>
+  </si>
+  <si>
+    <t>GOTO 6</t>
+  </si>
+  <si>
+    <t>if r4 == r0 then EXIT else GOTO 6</t>
+  </si>
+  <si>
+    <t>START HERE</t>
+  </si>
+  <si>
+    <t>&lt;-- main loop comes to here</t>
+  </si>
+  <si>
+    <t>r5 = 256 &gt; r1 ? 1 : 0</t>
+  </si>
+  <si>
+    <t>GOTO 18</t>
+  </si>
+  <si>
+    <t>if r1 &lt; 256 then GOTO 28 else GOTO 17</t>
   </si>
 </sst>
 </file>
@@ -554,24 +590,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F175A4B5-49A0-45DD-8E17-D2F2B838BD8D}">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="17.796875" customWidth="1"/>
-    <col min="3" max="3" width="18.1328125" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="6" max="6" width="16.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>0</v>
       </c>
@@ -582,7 +619,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>1</v>
       </c>
@@ -593,7 +630,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>2</v>
       </c>
@@ -607,7 +644,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>3</v>
       </c>
@@ -619,7 +656,7 @@
       </c>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>4</v>
       </c>
@@ -633,7 +670,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>5</v>
       </c>
@@ -643,8 +680,11 @@
       <c r="C7" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="D7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>6</v>
       </c>
@@ -654,8 +694,15 @@
       <c r="C8" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="D8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G8" t="str">
+        <f>_xlfn.CONCAT("s_",A8, ": i++; ", C8, ";")</f>
+        <v>s_6: i++; r1 = r4 | 65536 (0x10000);</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>7</v>
       </c>
@@ -665,8 +712,12 @@
       <c r="C9" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="G9" t="str">
+        <f t="shared" ref="G9:G32" si="0">_xlfn.CONCAT("s_",A9, ": i++; ", C9, ";")</f>
+        <v>s_7: i++; r4 = 678134;</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>8</v>
       </c>
@@ -676,8 +727,12 @@
       <c r="C10" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="G10" t="str">
+        <f t="shared" si="0"/>
+        <v>s_8: i++; r5 = r1 &amp; 255 (0xff);</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>9</v>
       </c>
@@ -687,8 +742,12 @@
       <c r="C11" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="G11" t="str">
+        <f t="shared" si="0"/>
+        <v>s_9: i++; r4 += r5;</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>10</v>
       </c>
@@ -698,8 +757,12 @@
       <c r="C12" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="G12" t="str">
+        <f t="shared" si="0"/>
+        <v>s_10: i++; r4 &amp;= 16777215 (0xffffff);</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>11</v>
       </c>
@@ -709,8 +772,12 @@
       <c r="C13" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="G13" t="str">
+        <f t="shared" si="0"/>
+        <v>s_11: i++; r4 *= 65899;</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>12</v>
       </c>
@@ -720,8 +787,12 @@
       <c r="C14" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="G14" t="str">
+        <f t="shared" si="0"/>
+        <v>s_12: i++; r4 &amp;= 16777215 (0xffffff);</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>13</v>
       </c>
@@ -729,13 +800,17 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="D15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>63</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="0"/>
+        <v>s_13: i++; r5 = 256 &gt; r1 ? 1 : 0;</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>14</v>
       </c>
@@ -743,10 +818,14 @@
         <v>14</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>43</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="0"/>
+        <v>s_14: i++; IP += r5;</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17">
         <v>15</v>
       </c>
@@ -756,8 +835,12 @@
       <c r="C17" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="G17" t="str">
+        <f t="shared" si="0"/>
+        <v>s_15: i++; IP ++;</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18">
         <v>16</v>
       </c>
@@ -767,8 +850,12 @@
       <c r="C18" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="G18" t="str">
+        <f t="shared" si="0"/>
+        <v>s_16: i++; GOTO 28;</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19">
         <v>17</v>
       </c>
@@ -776,10 +863,14 @@
         <v>17</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>47</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="0"/>
+        <v>s_17: i++; r5 = 0;</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20">
         <v>18</v>
       </c>
@@ -787,10 +878,14 @@
         <v>18</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>48</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="0"/>
+        <v>s_18: i++; r2 = r5 + 1;</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21">
         <v>19</v>
       </c>
@@ -798,10 +893,14 @@
         <v>19</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>49</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="0"/>
+        <v>s_19: i++; r2 *= 256;</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22">
         <v>20</v>
       </c>
@@ -809,87 +908,167 @@
         <v>20</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+        <v>50</v>
+      </c>
+      <c r="D22" t="s">
+        <v>52</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="0"/>
+        <v>s_20: i++; r2 = r2 &gt; r1 ? 1 : 0;</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="C23" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="0"/>
+        <v>s_21: i++; IP += r2;</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
+      <c r="C24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="0"/>
+        <v>s_22: i++; IP ++;</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
+      <c r="C25" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="0"/>
+        <v>s_23: i++; GOTO 26;</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="27" spans="1:3">
+      <c r="C26" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="0"/>
+        <v>s_24: i++; r5++;</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="28" spans="1:3">
+      <c r="C27" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="0"/>
+        <v>s_25: i++; GOTO 18;</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
+      <c r="C28" t="s">
+        <v>54</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="0"/>
+        <v>s_26: i++; r1 = r5;</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="30" spans="1:3">
+      <c r="C29" t="s">
+        <v>55</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="0"/>
+        <v>s_27: i++; GOTO 8;</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30">
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="31" spans="1:3">
+      <c r="C30" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D30" t="s">
+        <v>58</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="0"/>
+        <v>s_28: i++; r5 = r4 == r0 ? 1 : 0;</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31">
         <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="32" spans="1:3">
+      <c r="C31" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="0"/>
+        <v>s_29: i++; IP += r5;</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32">
         <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>28</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="0"/>
+        <v>s_30: i++; GOTO 6;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>